<commit_message>
[PHOENIX-6503] UI : Added the category details in asset service feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/assetDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/assetDetailsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="assetCategoryDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -561,6 +561,9 @@
     <t xml:space="preserve">ENGINEERING</t>
   </si>
   <si>
+    <t xml:space="preserve">Land</t>
+  </si>
+  <si>
     <t xml:space="preserve">01/04/2017</t>
   </si>
   <si>
@@ -571,9 +574,6 @@
   </si>
   <si>
     <t xml:space="preserve">REVENUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land</t>
   </si>
   <si>
     <t xml:space="preserve">01/04/2018</t>
@@ -839,17 +839,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="257" min="11" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="11" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1024,7 +1024,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1045,17 +1045,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="257" min="10" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="257" min="10" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1095,6 +1095,7 @@
         <v>41</v>
       </c>
       <c r="D2" s="2"/>
+      <c r="E2" s="0"/>
       <c r="G2" s="5" t="n">
         <v>1</v>
       </c>
@@ -1112,6 +1113,7 @@
       <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E3" s="0"/>
       <c r="G3" s="5" t="n">
         <v>2</v>
       </c>
@@ -1129,6 +1131,7 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E4" s="0"/>
       <c r="G4" s="5" t="n">
         <v>3</v>
       </c>
@@ -1146,6 +1149,7 @@
       <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E5" s="0"/>
       <c r="G5" s="5" t="n">
         <v>4</v>
       </c>
@@ -1163,6 +1167,7 @@
       <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E6" s="0"/>
       <c r="G6" s="5" t="n">
         <v>5</v>
       </c>
@@ -1180,6 +1185,7 @@
       <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E7" s="0"/>
       <c r="G7" s="5" t="n">
         <v>6</v>
       </c>
@@ -1198,6 +1204,7 @@
       <c r="C8" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E8" s="0"/>
       <c r="G8" s="5" t="n">
         <v>7</v>
       </c>
@@ -1216,6 +1223,7 @@
       <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E9" s="0"/>
       <c r="G9" s="5" t="n">
         <v>8</v>
       </c>
@@ -1234,6 +1242,7 @@
       <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E10" s="0"/>
       <c r="G10" s="5" t="n">
         <v>9</v>
       </c>
@@ -1252,6 +1261,7 @@
       <c r="C11" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E11" s="0"/>
       <c r="G11" s="5" t="n">
         <v>10</v>
       </c>
@@ -1270,6 +1280,7 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E12" s="0"/>
       <c r="G12" s="5" t="n">
         <v>11</v>
       </c>
@@ -1288,6 +1299,7 @@
       <c r="C13" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E13" s="0"/>
       <c r="G13" s="5" t="n">
         <v>11</v>
       </c>
@@ -1306,6 +1318,7 @@
       <c r="C14" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E14" s="0"/>
       <c r="G14" s="5" t="n">
         <v>12</v>
       </c>
@@ -1324,6 +1337,7 @@
       <c r="C15" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E15" s="0"/>
       <c r="G15" s="5" t="n">
         <v>13</v>
       </c>
@@ -1342,6 +1356,7 @@
       <c r="C16" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E16" s="0"/>
       <c r="G16" s="5" t="n">
         <v>14</v>
       </c>
@@ -1360,6 +1375,7 @@
       <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E17" s="0"/>
       <c r="G17" s="5" t="n">
         <v>15</v>
       </c>
@@ -1378,6 +1394,7 @@
       <c r="C18" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E18" s="0"/>
       <c r="G18" s="5" t="n">
         <v>16</v>
       </c>
@@ -1457,6 +1474,7 @@
       <c r="C22" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="E22" s="0"/>
       <c r="G22" s="5" t="n">
         <v>20</v>
       </c>
@@ -1475,6 +1493,7 @@
       <c r="C23" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E23" s="0"/>
       <c r="G23" s="5" t="n">
         <v>21</v>
       </c>
@@ -1493,6 +1512,7 @@
       <c r="C24" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E24" s="0"/>
       <c r="G24" s="5" t="n">
         <v>22</v>
       </c>
@@ -1511,6 +1531,7 @@
       <c r="C25" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="E25" s="0"/>
       <c r="G25" s="5" t="n">
         <v>23</v>
       </c>
@@ -1529,6 +1550,7 @@
       <c r="C26" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="E26" s="0"/>
       <c r="G26" s="5" t="n">
         <v>24</v>
       </c>
@@ -1547,6 +1569,7 @@
       <c r="C27" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="E27" s="0"/>
       <c r="G27" s="5" t="n">
         <v>25</v>
       </c>
@@ -1565,6 +1588,7 @@
       <c r="C28" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E28" s="0"/>
       <c r="G28" s="5" t="n">
         <v>26</v>
       </c>
@@ -1583,6 +1607,7 @@
       <c r="C29" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E29" s="0"/>
       <c r="G29" s="5" t="n">
         <v>27</v>
       </c>
@@ -1637,6 +1662,7 @@
       <c r="B32" s="4" t="s">
         <v>108</v>
       </c>
+      <c r="C32" s="0"/>
       <c r="G32" s="5" t="n">
         <v>30</v>
       </c>
@@ -2490,7 +2516,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2506,18 +2532,17 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="255" min="6" style="8" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="256" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="255" min="6" style="8" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2545,24 +2570,24 @@
         <v>177</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>20</v>
+        <v>178</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>183</v>
@@ -2579,7 +2604,7 @@
         <v>186</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>17</v>
+        <v>178</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>187</v>
@@ -2591,7 +2616,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2612,12 +2637,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2691,7 +2714,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2711,9 +2734,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2750,7 +2770,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2771,9 +2791,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2811,7 +2829,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[EGSVC-42] - UI : Working on the Creating the agreement feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/assetDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/assetDetailsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="assetCategoryDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="239">
   <si>
     <t xml:space="preserve">dataRow</t>
   </si>
@@ -576,6 +576,9 @@
     <t xml:space="preserve">REVENUE</t>
   </si>
   <si>
+    <t xml:space="preserve">Market</t>
+  </si>
+  <si>
     <t xml:space="preserve">01/04/2018</t>
   </si>
   <si>
@@ -585,13 +588,79 @@
     <t xml:space="preserve">header3</t>
   </si>
   <si>
-    <t xml:space="preserve">Test</t>
+    <t xml:space="preserve">ACCOUNTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parking Space</t>
   </si>
   <si>
     <t xml:space="preserve">01/04/2019</t>
   </si>
   <si>
     <t xml:space="preserve">TENDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">header4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMINISTRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lakes and Ponds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/05/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DONATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">header5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/05/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">header6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUBLIC HEALTH AND SANITATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Community Toilet Complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/05/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">header7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOWN PLANNING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usufruct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/05/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PURCHASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">header8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URBAN POVERTY ALLEVIATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Street light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/05/2021</t>
   </si>
   <si>
     <t xml:space="preserve">location</t>
@@ -768,7 +837,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -805,11 +874,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -834,10 +907,10 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.9030612244898"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0867346938776"/>
@@ -852,7 +925,7 @@
     <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -884,7 +957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -898,7 +971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -912,7 +985,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -926,7 +999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -940,7 +1013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -954,7 +1027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -968,7 +1041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -982,7 +1055,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -996,7 +1069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1010,7 +1083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1039,11 +1112,11 @@
   </sheetPr>
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H80" activeCellId="0" sqref="H80"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CN17" activeCellId="0" sqref="CN17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.219387755102"/>
@@ -1058,7 +1131,7 @@
     <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1157,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
@@ -1095,7 +1168,6 @@
         <v>41</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="0"/>
       <c r="G2" s="5" t="n">
         <v>1</v>
       </c>
@@ -1103,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -1113,7 +1185,6 @@
       <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="0"/>
       <c r="G3" s="5" t="n">
         <v>2</v>
       </c>
@@ -1121,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -1131,7 +1202,6 @@
       <c r="C4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="0"/>
       <c r="G4" s="5" t="n">
         <v>3</v>
       </c>
@@ -1139,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>46</v>
       </c>
@@ -1149,7 +1219,6 @@
       <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="0"/>
       <c r="G5" s="5" t="n">
         <v>4</v>
       </c>
@@ -1157,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -1167,7 +1236,6 @@
       <c r="C6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="0"/>
       <c r="G6" s="5" t="n">
         <v>5</v>
       </c>
@@ -1175,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -1185,7 +1253,6 @@
       <c r="C7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="0"/>
       <c r="G7" s="5" t="n">
         <v>6</v>
       </c>
@@ -1194,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
@@ -1204,7 +1271,6 @@
       <c r="C8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="0"/>
       <c r="G8" s="5" t="n">
         <v>7</v>
       </c>
@@ -1213,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -1223,7 +1289,6 @@
       <c r="C9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="0"/>
       <c r="G9" s="5" t="n">
         <v>8</v>
       </c>
@@ -1232,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>56</v>
       </c>
@@ -1242,7 +1307,6 @@
       <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="0"/>
       <c r="G10" s="5" t="n">
         <v>9</v>
       </c>
@@ -1251,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
@@ -1261,7 +1325,6 @@
       <c r="C11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="0"/>
       <c r="G11" s="5" t="n">
         <v>10</v>
       </c>
@@ -1270,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>60</v>
       </c>
@@ -1280,7 +1343,6 @@
       <c r="C12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="0"/>
       <c r="G12" s="5" t="n">
         <v>11</v>
       </c>
@@ -1289,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>63</v>
       </c>
@@ -1299,7 +1361,6 @@
       <c r="C13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="0"/>
       <c r="G13" s="5" t="n">
         <v>11</v>
       </c>
@@ -1308,7 +1369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>65</v>
       </c>
@@ -1318,7 +1379,6 @@
       <c r="C14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="0"/>
       <c r="G14" s="5" t="n">
         <v>12</v>
       </c>
@@ -1327,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>67</v>
       </c>
@@ -1337,7 +1397,6 @@
       <c r="C15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="0"/>
       <c r="G15" s="5" t="n">
         <v>13</v>
       </c>
@@ -1346,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>69</v>
       </c>
@@ -1356,7 +1415,6 @@
       <c r="C16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="0"/>
       <c r="G16" s="5" t="n">
         <v>14</v>
       </c>
@@ -1365,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>71</v>
       </c>
@@ -1375,7 +1433,6 @@
       <c r="C17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="0"/>
       <c r="G17" s="5" t="n">
         <v>15</v>
       </c>
@@ -1384,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>73</v>
       </c>
@@ -1394,7 +1451,6 @@
       <c r="C18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="0"/>
       <c r="G18" s="5" t="n">
         <v>16</v>
       </c>
@@ -1403,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
@@ -1424,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>79</v>
       </c>
@@ -1444,7 +1500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>82</v>
       </c>
@@ -1464,7 +1520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>85</v>
       </c>
@@ -1474,7 +1530,6 @@
       <c r="C22" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="0"/>
       <c r="G22" s="5" t="n">
         <v>20</v>
       </c>
@@ -1483,7 +1538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>87</v>
       </c>
@@ -1493,7 +1548,6 @@
       <c r="C23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E23" s="0"/>
       <c r="G23" s="5" t="n">
         <v>21</v>
       </c>
@@ -1502,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>89</v>
       </c>
@@ -1512,7 +1566,6 @@
       <c r="C24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="0"/>
       <c r="G24" s="5" t="n">
         <v>22</v>
       </c>
@@ -1521,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>91</v>
       </c>
@@ -1531,7 +1584,6 @@
       <c r="C25" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="0"/>
       <c r="G25" s="5" t="n">
         <v>23</v>
       </c>
@@ -1540,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>94</v>
       </c>
@@ -1550,7 +1602,6 @@
       <c r="C26" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="0"/>
       <c r="G26" s="5" t="n">
         <v>24</v>
       </c>
@@ -1559,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>96</v>
       </c>
@@ -1569,7 +1620,6 @@
       <c r="C27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E27" s="0"/>
       <c r="G27" s="5" t="n">
         <v>25</v>
       </c>
@@ -1578,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>98</v>
       </c>
@@ -1588,7 +1638,6 @@
       <c r="C28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="0"/>
       <c r="G28" s="5" t="n">
         <v>26</v>
       </c>
@@ -1597,7 +1646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>100</v>
       </c>
@@ -1607,7 +1656,6 @@
       <c r="C29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="0"/>
       <c r="G29" s="5" t="n">
         <v>27</v>
       </c>
@@ -1616,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>102</v>
       </c>
@@ -1637,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>105</v>
       </c>
@@ -1655,14 +1703,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="0"/>
       <c r="G32" s="5" t="n">
         <v>30</v>
       </c>
@@ -1671,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>109</v>
       </c>
@@ -1688,7 +1735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>111</v>
       </c>
@@ -1705,7 +1752,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>113</v>
       </c>
@@ -1722,7 +1769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>115</v>
       </c>
@@ -1739,7 +1786,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>117</v>
       </c>
@@ -1757,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>119</v>
       </c>
@@ -1775,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>120</v>
       </c>
@@ -1793,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>121</v>
       </c>
@@ -1811,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>122</v>
       </c>
@@ -1829,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>123</v>
       </c>
@@ -1847,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>124</v>
       </c>
@@ -1865,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>126</v>
       </c>
@@ -1883,7 +1930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>127</v>
       </c>
@@ -1901,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>128</v>
       </c>
@@ -1919,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>129</v>
       </c>
@@ -1937,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>130</v>
       </c>
@@ -1955,7 +2002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>131</v>
       </c>
@@ -1973,7 +2020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>133</v>
       </c>
@@ -1991,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>134</v>
       </c>
@@ -2009,7 +2056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>135</v>
       </c>
@@ -2027,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>136</v>
       </c>
@@ -2045,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>137</v>
       </c>
@@ -2063,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>138</v>
       </c>
@@ -2081,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>140</v>
       </c>
@@ -2099,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>141</v>
       </c>
@@ -2117,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>142</v>
       </c>
@@ -2135,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>143</v>
       </c>
@@ -2153,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>144</v>
       </c>
@@ -2171,7 +2218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
@@ -2189,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>147</v>
       </c>
@@ -2207,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
         <v>148</v>
       </c>
@@ -2225,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
         <v>149</v>
       </c>
@@ -2243,7 +2290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>150</v>
       </c>
@@ -2261,7 +2308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>151</v>
       </c>
@@ -2279,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
         <v>152</v>
       </c>
@@ -2297,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
         <v>154</v>
       </c>
@@ -2315,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
         <v>155</v>
       </c>
@@ -2333,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
         <v>156</v>
       </c>
@@ -2351,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
         <v>157</v>
       </c>
@@ -2369,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
         <v>158</v>
       </c>
@@ -2387,7 +2434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
         <v>159</v>
       </c>
@@ -2405,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
         <v>161</v>
       </c>
@@ -2423,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
         <v>162</v>
       </c>
@@ -2441,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
         <v>164</v>
       </c>
@@ -2459,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>166</v>
       </c>
@@ -2477,7 +2524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
         <v>168</v>
       </c>
@@ -2495,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
         <v>170</v>
       </c>
@@ -2529,23 +2576,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="8" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="31.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="23.6683673469388"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="8" width="13.9030612244898"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="8" width="17.5510204081633"/>
     <col collapsed="false" hidden="false" max="255" min="6" style="8" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="256" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2562,7 +2610,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>176</v>
       </c>
@@ -2579,7 +2627,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>181</v>
       </c>
@@ -2587,30 +2635,115 @@
         <v>182</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>188</v>
+    </row>
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2632,83 +2765,85 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.6734693877551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.280612244898"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>189</v>
+        <v>212</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>191</v>
+        <v>214</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>193</v>
+        <v>216</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>194</v>
+        <v>217</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>201</v>
+        <v>224</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2729,41 +2864,44 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>205</v>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2786,44 +2924,46 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>209</v>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>211</v>
+      <c r="A2" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>213</v>
+      <c r="A3" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>215</v>
+      <c r="A4" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>